<commit_message>
temporary removal of forward slashes for erd test
</commit_message>
<xml_diff>
--- a/examples/clover3d/genesis_datacard.xlsx
+++ b/examples/clover3d/genesis_datacard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Shared/dev/dsi/examples/clover3d/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C83950F8-F7A2-8E42-9F11-749CBB798435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D030E9A5-1750-FF44-969A-CBC3D4E910D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="1320" windowWidth="27640" windowHeight="16940" xr2:uid="{ACA5C62D-F69A-9A41-B523-772E0840A19D}"/>
   </bookViews>
@@ -89,9 +89,6 @@
     <t>DCAT-US - Version 3 - Dataset Title</t>
   </si>
   <si>
-    <t>Keywords/Tag</t>
-  </si>
-  <si>
     <t>Tags (or keywords) help users discover your dataset; please include terms that would be used by technical and non-technical users.</t>
   </si>
   <si>
@@ -108,9 +105,6 @@
   </si>
   <si>
     <t>"This property contains a keyword or tag describing the Dataset. Good practice: mark the language of the keywords with the [ISO 639-1] language code such as ""geodata""@en."</t>
-  </si>
-  <si>
-    <t>Update/Modification Date</t>
   </si>
   <si>
     <t>Most recent date on which the dataset was changed, updated or modified.</t>
@@ -136,9 +130,6 @@
 For example, September 27, 2022 at 6 p.m. is represented as 2022-09-27 18:00:00.000.</t>
   </si>
   <si>
-    <t>Theme/Category : Domain</t>
-  </si>
-  <si>
     <t>The conceptual domain in which the dataset, governance, and data stewards reside.</t>
   </si>
   <si>
@@ -263,6 +254,15 @@
   </si>
   <si>
     <t>pulido@lanl.gov</t>
+  </si>
+  <si>
+    <t>Keywords_Tag</t>
+  </si>
+  <si>
+    <t>Update_Modification Date</t>
+  </si>
+  <si>
+    <t>Theme_Category : Domain</t>
   </si>
 </sst>
 </file>
@@ -746,7 +746,7 @@
   <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -803,7 +803,7 @@
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>15</v>
@@ -817,109 +817,109 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>17</v>
+        <v>70</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="8" t="s">
+      <c r="F3" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="G3" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="H3" s="5" t="s">
+      <c r="I3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="J3" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>23</v>
       </c>
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>24</v>
+        <v>71</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="8" t="s">
         <v>25</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>27</v>
       </c>
       <c r="G4" s="9">
         <v>45939</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K4" s="5"/>
       <c r="L4" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>31</v>
+        <v>72</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="8" t="s">
+      <c r="H5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="J5" s="5" t="s">
         <v>34</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>37</v>
       </c>
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B6" s="10"/>
       <c r="C6" s="10" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>13</v>
@@ -928,51 +928,51 @@
         <v>14</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="K6" s="11"/>
       <c r="L6" s="11"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>13</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
@@ -980,23 +980,23 @@
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="B8" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>13</v>
       </c>
       <c r="E8" s="8"/>
       <c r="F8" s="8" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G8" s="16" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I8" s="6"/>
       <c r="J8" s="5"/>
@@ -1006,23 +1006,23 @@
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="B9" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>13</v>
       </c>
       <c r="E9" s="8"/>
       <c r="F9" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I9" s="6"/>
       <c r="J9" s="5"/>
@@ -1031,62 +1031,62 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>13</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="K10" s="7"/>
       <c r="L10" s="5"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="J11" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>59</v>
       </c>
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
@@ -1094,10 +1094,10 @@
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>13</v>
@@ -1105,10 +1105,10 @@
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
@@ -1118,10 +1118,10 @@
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" s="13" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>13</v>
@@ -1129,21 +1129,21 @@
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
       <c r="G13" s="8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I13" s="5"/>
       <c r="J13" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B14" s="14"/>
       <c r="C14" s="14"/>
@@ -1151,11 +1151,11 @@
         <v>13</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F14" s="14"/>
       <c r="G14" s="14" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="H14" s="14"/>
       <c r="I14" s="14"/>

</xml_diff>